<commit_message>
Download county election results; update notes.
</commit_message>
<xml_diff>
--- a/Bishops_and_dioceses_Roman.xlsx
+++ b/Bishops_and_dioceses_Roman.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acavender/Documents/Data analysis/bishopsAndTwitter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27164034-3D5D-E446-BDFD-F37ECD2C182B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963816A9-C30E-064D-A91E-E7EE84A8546A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D8E070FD-0820-4B8C-90FF-3D3990EBEDA3}"/>
   </bookViews>
@@ -4099,7 +4099,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4123,7 +4123,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4442,8 +4441,8 @@
   <dimension ref="A1:AB415"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H326" sqref="H326"/>
+      <pane ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19189,7 +19188,7 @@
       <c r="G326" t="s">
         <v>24</v>
       </c>
-      <c r="H326" s="13" t="s">
+      <c r="H326" t="s">
         <v>1257</v>
       </c>
       <c r="I326" s="7" t="s">

</xml_diff>